<commit_message>
Updating build and adding Create JSONs
</commit_message>
<xml_diff>
--- a/top_250_data.xlsx
+++ b/top_250_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C262"/>
+  <dimension ref="A1:C263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4356,14 +4356,29 @@
           <t>Attack on Titan: Wings of Freedom</t>
         </is>
       </c>
-      <c r="B262" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
+      <c r="B262" t="n">
+        <v>2015</v>
       </c>
       <c r="C262" t="inlineStr">
         <is>
           <t>https://letterboxd.com/film/attack-on-titan-wings-of-freedom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>One Battle After Another</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/one-battle-after-another/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some errors in updating lists and scraping genres
</commit_message>
<xml_diff>
--- a/top_250_data.xlsx
+++ b/top_250_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C266"/>
+  <dimension ref="A1:C267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4416,14 +4416,29 @@
           <t>National Theatre Live: Inter Alia</t>
         </is>
       </c>
-      <c r="B266" t="inlineStr">
+      <c r="B266" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/national-theatre-live-inter-alia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Chainsaw Man – The Movie: Reze Arc</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
         <is>
           <t>2025</t>
         </is>
       </c>
-      <c r="C266" t="inlineStr">
-        <is>
-          <t>https://letterboxd.com/film/national-theatre-live-inter-alia/</t>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/chainsaw-man-the-movie-reze-arc/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new pronoun lists from Letterboxd
</commit_message>
<xml_diff>
--- a/top_250_data.xlsx
+++ b/top_250_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C268"/>
+  <dimension ref="A1:C269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4446,14 +4446,29 @@
           <t>Nirvanna the Band the Show the Movie</t>
         </is>
       </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
+      <c r="B268" t="n">
+        <v>2025</v>
       </c>
       <c r="C268" t="inlineStr">
         <is>
           <t>https://letterboxd.com/film/nirvanna-the-band-the-show-the-movie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Streetwise</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>1984</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>https://letterboxd.com/film/streetwise/</t>
         </is>
       </c>
     </row>

</xml_diff>